<commit_message>
Need to Proof Report
Mick is finishing off manual :)
</commit_message>
<xml_diff>
--- a/CTM - Operational Images/current meter calibrations.xlsx
+++ b/CTM - Operational Images/current meter calibrations.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c07c9239cf8ef362/4th Year Sem2/CC3501/Github/CT-Monitoring-Assignment/Data Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clint\OneDrive\4th Year Sem2\CC3501\Github\CT-Monitoring-Assignment\CTM - Operational Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="27" documentId="09478EAF7D65D97B38BF161B9D4F54A951446D3B" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{87DB52EA-33B9-41F3-BD57-40A682D0E0BC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8556" xr2:uid="{0CBA6DDC-5F93-426C-A027-5223CDC0C121}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8556" xr2:uid="{0CBA6DDC-5F93-426C-A027-5223CDC0C121}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,21 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>amp</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>avg</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>amp/avg</t>
   </si>
   <si>
     <t>avg/amp</t>
+  </si>
+  <si>
+    <t>Verifed Current</t>
+  </si>
+  <si>
+    <t>Percentage Scaled From Kinetis</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>CT % Avg</t>
+  </si>
+  <si>
+    <t>Amp/CT%Avg</t>
+  </si>
+  <si>
+    <t>Verifed Amps</t>
+  </si>
+  <si>
+    <t>Scaling Factor</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
@@ -74,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,32 +407,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94DD8F2-D970-49AB-866D-695BFCFF814A}">
-  <dimension ref="C3:L29"/>
+  <dimension ref="C3:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="N5" sqref="N5:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>0.2</v>
       </c>
@@ -435,19 +469,28 @@
         <v>1.39</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I5:I7" si="0">SUM(D6:H6)/5</f>
+        <f t="shared" ref="I6:I7" si="0">SUM(D6:H6)/5</f>
         <v>1.3679999999999999</v>
       </c>
-      <c r="K6">
+      <c r="J6">
         <f>C6/I6</f>
         <v>0.14619883040935674</v>
       </c>
-      <c r="L6">
-        <f t="shared" ref="L5:L7" si="1">I6/C6</f>
+      <c r="K6">
+        <f t="shared" ref="K6:K7" si="1">I6/C6</f>
         <v>6.839999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="N6">
+        <v>0.2</v>
+      </c>
+      <c r="O6">
+        <v>1.3679999999999999</v>
+      </c>
+      <c r="P6">
+        <v>0.14619883040935674</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>0.2</v>
       </c>
@@ -470,16 +513,36 @@
         <f t="shared" si="0"/>
         <v>1.2819999999999998</v>
       </c>
+      <c r="J7">
+        <f t="shared" ref="J7" si="2">C7/I7</f>
+        <v>0.15600624024961002</v>
+      </c>
       <c r="K7">
-        <f t="shared" ref="K5:K7" si="2">C7/I7</f>
-        <v>0.15600624024961002</v>
-      </c>
-      <c r="L7">
         <f t="shared" si="1"/>
         <v>6.4099999999999984</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="N7">
+        <v>0.2</v>
+      </c>
+      <c r="O7">
+        <v>1.2819999999999998</v>
+      </c>
+      <c r="P7">
+        <v>0.15600624024961002</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="N8">
+        <v>0.5</v>
+      </c>
+      <c r="O8">
+        <v>3.3379999999999996</v>
+      </c>
+      <c r="P8">
+        <v>0.14979029358897544</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>0.5</v>
       </c>
@@ -502,16 +565,25 @@
         <f t="shared" ref="I9" si="3">SUM(D9:H9)/5</f>
         <v>3.3379999999999996</v>
       </c>
+      <c r="J9">
+        <f t="shared" ref="J9" si="4">C9/I9</f>
+        <v>0.14979029358897544</v>
+      </c>
       <c r="K9">
-        <f t="shared" ref="K9" si="4">C9/I9</f>
-        <v>0.14979029358897544</v>
-      </c>
-      <c r="L9">
-        <f t="shared" ref="L9" si="5">I9/C9</f>
+        <f t="shared" ref="K9" si="5">I9/C9</f>
         <v>6.6759999999999993</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>0.5</v>
+      </c>
+      <c r="O9">
+        <v>3.3220000000000001</v>
+      </c>
+      <c r="P9">
+        <v>0.15051173991571343</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>0.5</v>
       </c>
@@ -534,34 +606,63 @@
         <f t="shared" ref="I10" si="6">SUM(D10:H10)/5</f>
         <v>3.3220000000000001</v>
       </c>
+      <c r="J10">
+        <f t="shared" ref="J10" si="7">C10/I10</f>
+        <v>0.15051173991571343</v>
+      </c>
       <c r="K10">
-        <f t="shared" ref="K10" si="7">C10/I10</f>
-        <v>0.15051173991571343</v>
-      </c>
-      <c r="L10">
-        <f t="shared" ref="L10" si="8">I10/C10</f>
+        <f t="shared" ref="K10" si="8">I10/C10</f>
         <v>6.6440000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="O10">
+        <v>48.808000000000007</v>
+      </c>
+      <c r="P10">
+        <v>0.18029831175217176</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.3">
       <c r="I11">
         <f t="shared" ref="I11:I29" si="9">SUM(D11:H11)/5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="N11">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="O11">
+        <v>49.044000000000004</v>
+      </c>
+      <c r="P11">
+        <v>0.17943071527607862</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="N12" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12">
+        <v>0.1603726885319843</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.3">
       <c r="I13">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.3">
       <c r="I14">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>8.8000000000000007</v>
       </c>
@@ -584,22 +685,22 @@
         <f t="shared" si="9"/>
         <v>48.808000000000007</v>
       </c>
+      <c r="J15">
+        <f t="shared" ref="J15" si="10">C15/I15</f>
+        <v>0.18029831175217176</v>
+      </c>
       <c r="K15">
-        <f t="shared" ref="K15" si="10">C15/I15</f>
-        <v>0.18029831175217176</v>
-      </c>
-      <c r="L15">
-        <f t="shared" ref="L15" si="11">I15/C15</f>
+        <f t="shared" ref="K15" si="11">I15/C15</f>
         <v>5.5463636363636368</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.3">
       <c r="I16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>8.8000000000000007</v>
       </c>
@@ -622,86 +723,86 @@
         <f t="shared" si="9"/>
         <v>49.044000000000004</v>
       </c>
+      <c r="J17">
+        <f t="shared" ref="J17" si="12">C17/I17</f>
+        <v>0.17943071527607862</v>
+      </c>
       <c r="K17">
-        <f t="shared" ref="K17" si="12">C17/I17</f>
-        <v>0.17943071527607862</v>
-      </c>
-      <c r="L17">
-        <f t="shared" ref="L17" si="13">I17/C17</f>
+        <f t="shared" ref="K17" si="13">I17/C17</f>
         <v>5.5731818181818182</v>
       </c>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I18">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I19">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I20">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K20">
-        <f>SUM(K6:K17)/6</f>
+      <c r="J20">
+        <f>SUM(J6:J17)/6</f>
         <v>0.1603726885319843</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I21">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I22">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I23">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I24">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I25">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I26">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I27">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
       <c r="I29">
         <f t="shared" si="9"/>
         <v>0</v>

</xml_diff>